<commit_message>
Add: Process, Release and Object of Address Book System
</commit_message>
<xml_diff>
--- a/ContactsExcelFile.xlsx
+++ b/ContactsExcelFile.xlsx
@@ -96,12 +96,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,14 +120,6 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -136,57 +128,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -201,6 +142,45 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -208,6 +188,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -217,23 +204,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -241,13 +227,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -261,9 +240,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -278,19 +271,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -302,163 +433,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -472,17 +465,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -498,15 +485,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -531,6 +509,21 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -574,161 +567,158 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1051,7 +1041,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="3"/>
@@ -1092,7 +1082,7 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5"/>
+      <c r="I1" s="1"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
@@ -1119,8 +1109,8 @@
       <c r="H2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
@@ -1144,11 +1134,11 @@
       <c r="G3" s="1">
         <v>8745214789</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
@@ -1172,11 +1162,11 @@
       <c r="G4" s="1">
         <v>7858965478</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>